<commit_message>
MS: fixing issue #26
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@123 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
+++ b/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="2" r:id="rId1"/>
     <sheet name="Test2" sheetId="1" r:id="rId2"/>
     <sheet name="Test3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>NumericColumn</t>
   </si>
@@ -34,6 +35,60 @@
   </si>
   <si>
     <t>World</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -387,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F11:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -615,4 +670,124 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D8:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="8" spans="4:7">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7">
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7">
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7">
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7">
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7">
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MS: moving to 3.8-beta4; extending saveWorkbook to be able to save workbook to different file ("save as"); fix for determination of bounding box when using readWorksheet (+ unit tests)
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@127 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
+++ b/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="2" r:id="rId1"/>
     <sheet name="Test2" sheetId="1" r:id="rId2"/>
     <sheet name="Test3" sheetId="3" r:id="rId3"/>
     <sheet name="Test4" sheetId="4" r:id="rId4"/>
+    <sheet name="Test5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>NumericColumn</t>
   </si>
@@ -676,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D8:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -790,4 +791,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="F17:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="17" spans="6:9">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9">
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9">
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9">
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9">
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9">
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9">
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9">
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9">
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MS: getBounding, readWorksheet; switching to UTF-8 encoding for unit tests
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@298 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
+++ b/inst/unitTests/resources/testWorkbookReadWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="8"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="AAA" sheetId="7" r:id="rId7"/>
     <sheet name="BBB" sheetId="8" r:id="rId8"/>
     <sheet name="VariableNames" sheetId="9" r:id="rId9"/>
+    <sheet name="BoundingBox" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -580,6 +581,74 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C7:R33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7" spans="4:16">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16">
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18">
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18">
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18">
+      <c r="L28">
+        <v>11</v>
+      </c>
+      <c r="N28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D5:I22"/>
@@ -970,7 +1039,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1183,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>